<commit_message>
Refactor routing and controller logic, add middleware and ML insights endpoint
</commit_message>
<xml_diff>
--- a/backend/exports/transactions.xlsx
+++ b/backend/exports/transactions.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="38">
   <si>
     <t>Date</t>
   </si>
@@ -97,6 +97,9 @@
     <t>456.00</t>
   </si>
   <si>
+    <t>fdgdfgwaegrgrg</t>
+  </si>
+  <si>
     <t>fyfyuftyj</t>
   </si>
   <si>
@@ -113,6 +116,12 @@
   </si>
   <si>
     <t>transaction added by user</t>
+  </si>
+  <si>
+    <t>45.00</t>
+  </si>
+  <si>
+    <t>rent</t>
   </si>
   <si>
     <t>added by user</t>
@@ -493,7 +502,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E15"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="2" width="20" customWidth="1"/>
@@ -640,7 +649,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>45792.875</v>
+        <v>45796.875</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
@@ -652,58 +661,109 @@
         <v>28</v>
       </c>
       <c r="E9" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>45789.875</v>
+        <v>45792.875</v>
       </c>
       <c r="B10" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" t="s">
         <v>29</v>
       </c>
-      <c r="D10" t="s">
-        <v>30</v>
-      </c>
       <c r="E10" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>45782.875</v>
+        <v>45789.875</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="C11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" t="s">
         <v>32</v>
-      </c>
-      <c r="D11" t="s">
-        <v>33</v>
-      </c>
-      <c r="E11" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>45762.875</v>
+        <v>45782.875</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C12" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="D12" t="s">
         <v>34</v>
       </c>
       <c r="E12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>45782.875</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" t="s">
         <v>31</v>
+      </c>
+      <c r="E13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>45774.875</v>
+      </c>
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>45762.875</v>
+      </c>
+      <c r="B15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" t="s">
+        <v>37</v>
+      </c>
+      <c r="E15" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>